<commit_message>
Mais POJOs e estrutura de pastas
</commit_message>
<xml_diff>
--- a/Normalizações do Projeto.xlsx
+++ b/Normalizações do Projeto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Elemento</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>private String nomeDoFuncionario</t>
+  </si>
+  <si>
+    <t>Tipos de Variável</t>
+  </si>
+  <si>
+    <t>Usar Wrappers ao invés de tipos primitos</t>
+  </si>
+  <si>
+    <t>private Integer id</t>
   </si>
   <si>
     <t>Classe</t>
@@ -424,16 +433,16 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
@@ -454,10 +463,10 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -466,10 +475,10 @@
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -493,21 +502,21 @@
       <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -519,21 +528,21 @@
       <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="D11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
@@ -542,12 +551,10 @@
       <c r="B13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="D13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
@@ -557,7 +564,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>41</v>
@@ -571,38 +578,52 @@
         <v>43</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>